<commit_message>
updated lab data dictionary
</commit_message>
<xml_diff>
--- a/SIAL_docs/SIAL_data_dictionary.xlsx
+++ b/SIAL_docs/SIAL_data_dictionary.xlsx
@@ -7040,8 +7040,8 @@
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7050,8 +7050,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="647700" y="6092188"/>
-          <a:ext cx="9420225" cy="5490212"/>
+          <a:off x="647700" y="6076948"/>
+          <a:ext cx="9420225" cy="7433312"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7375,9 +7375,7 @@
             </a:rPr>
             <a:t>See source data dictionary. As this is a reformatted table any underlying quality issues with the source data will remain in this table.</a:t>
           </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
+          <a:br>
             <a:rPr lang="en-NZ" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
@@ -7387,21 +7385,240 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Uncertainty of accuracy of information</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Due to out-of-date business rules, MOH know that a large number of laboratory claims are included in the data that shouldn't be. Conversely they know that a large number of claims are not included in the data that should be. For these reasons, MOH are uncertain of the accuracy of the overall volumes and cost. </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Bulk funded claims affect data quality</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>The funding of laboratory claims has changed over time from 'fee for service' (FFS) payment to bulk funding. Where the laboratory was bulk funded, the amount paid variable will be blank. In addition, the estimated amount paid variable will include an estimated amount paid for service providers that were bulk funded. MOH recommend that you use the 'estimated amount paid' variable instead of the amount paid variable. </a:t>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t/>
+          </a:r>
+          <a:br>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+          </a:br>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>It is important to note that the estimated amount is based on a 2010 value and requires updating. </a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NZ" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t> </a:t>
           </a:r>
         </a:p>
         <a:p>
           <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>High level details about some of the quality issues include:</a:t>
+            <a:rPr lang="en-NZ" sz="1100" b="1">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>Other quality notes</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -17902,7 +18119,7 @@
   </sheetPr>
   <dimension ref="B1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A21" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A39" workbookViewId="0">
       <selection activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
updated moh parts of data dictionary
</commit_message>
<xml_diff>
--- a/SIAL_docs/SIAL_data_dictionary.xlsx
+++ b/SIAL_docs/SIAL_data_dictionary.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="132" windowWidth="14880" windowHeight="7908" firstSheet="21" activeTab="26"/>
+    <workbookView xWindow="480" yWindow="132" windowWidth="14880" windowHeight="7908" tabRatio="842"/>
   </bookViews>
   <sheets>
     <sheet name="SIAL contents" sheetId="1" r:id="rId1"/>
@@ -5441,15 +5441,6 @@
             </a:rPr>
             <a:t>It is important to note that the estimated amount is based on a 2010 value and requires updating. </a:t>
           </a:r>
-          <a:endParaRPr lang="en-NZ" sz="1100">
-            <a:solidFill>
-              <a:schemeClr val="dk1"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:pPr eaLnBrk="1" fontAlgn="auto" latinLnBrk="0" hangingPunct="1"/>
@@ -7437,8 +7428,31 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Forensic services have not been costed due to a different funding mechanism for these.</a:t>
-          </a:r>
+            <a:t>Services</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> have been costed using mapped codes, budget and count information provided by MOH.  Using the PBFF information. This information was not intended for costing and will not reconcile to national level expenditure on mental health costs. Due to half complete data in the IDI, costing will not go back before July 2012.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:endParaRPr lang="en-NZ" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
         </a:p>
         <a:p>
           <a:r>
@@ -7583,6 +7597,17 @@
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
           </a:br>
+          <a:endParaRPr lang="en-NZ" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-NZ" sz="1100" b="1">
               <a:solidFill>
@@ -7593,8 +7618,10 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-            <a:t>Uncertainty of accuracy of information</a:t>
-          </a:r>
+            <a:t>Other quality notes</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
           <a:r>
             <a:rPr lang="en-NZ" sz="1100">
               <a:solidFill>
@@ -7605,9 +7632,231 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>1. In some cases data is missing or incomplete. There are a number of reasons for this. Some examples are:</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- The gradual uptake of reporting by NGOs to PRIMHD.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Regional differences in funding for older people's mental health services.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Gaps in reporting due to changes in organisation structures and systems.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- Diagnosis required</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> to be submitted within 3 month of treatment which means the diagnosis is not recorded particlarly for those who receieve short term treatment</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NZ" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> </a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>2. Changes in reporting practices over time can lead to variances in the data.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- there is a lot of variation within DHBs in terms of what is submitted and the quality of the data that is submitted</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>3. Inconsistent or miss-use of codes, including data entry errors.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>- there are a lot of non</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t> specific diagnoses such as 'diagnosis deferred' or 'no specific diagnosis'</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-NZ" sz="1100">
+            <a:solidFill>
+              <a:schemeClr val="dk1"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+          </a:endParaRPr>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>4. Organisations resubmit previously submitted data as necessary, for example to make data corrections. This means numbers can change over time.</a:t>
+          </a:r>
+        </a:p>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
+            <a:t>5. Some</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-NZ" sz="1100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="dk1"/>
+              </a:solidFill>
+              <a:effectLst/>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:rPr>
             <a:t> </a:t>
           </a:r>
-          <a:br>
+          <a:r>
             <a:rPr lang="en-NZ" sz="1100">
               <a:solidFill>
                 <a:schemeClr val="dk1"/>
@@ -7617,299 +7866,7 @@
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="+mn-cs"/>
             </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Due to out-of-date business rules, MOH know that a large number of laboratory claims are included in the data that shouldn't be. Conversely they know that a large number of claims are not included in the data that should be. For these reasons, MOH are uncertain of the accuracy of the overall volumes and cost. </a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-NZ" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Bulk funded claims affect data quality</a:t>
-          </a:r>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>The funding of laboratory claims has changed over time from 'fee for service' (FFS) payment to bulk funding. Where the laboratory was bulk funded, the amount paid variable will be blank. In addition, the estimated amount paid variable will include an estimated amount paid for service providers that were bulk funded. MOH recommend that you use the 'estimated amount paid' variable instead of the amount paid variable. </a:t>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t/>
-          </a:r>
-          <a:br>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-          </a:br>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>It is important to note that the estimated amount is based on a 2010 value and requires updating. </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100" b="1">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>Other quality notes</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>1. In some cases data is missing or incomplete. There are a number of reasons for this. Some examples are:</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- The gradual uptake of reporting by NGOs to PRIMHD.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Regional differences in funding for older people's mental health services.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>- Gaps in reporting due to changes in organisation structures and systems.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t> </a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>2. Changes in reporting practices over time can lead to variances in the data.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>3. Inconsistent or miss-use of codes, including data entry errors.</a:t>
-          </a:r>
-        </a:p>
-        <a:p>
-          <a:r>
-            <a:rPr lang="en-NZ" sz="1100">
-              <a:solidFill>
-                <a:schemeClr val="dk1"/>
-              </a:solidFill>
-              <a:effectLst/>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:rPr>
-            <a:t>4. Organisations resubmit previously submitted data as necessary, for example to make data corrections. This means numbers can change over time.</a:t>
+            <a:t>systems set the diagnosis date to the date the data was submitted rather than the diagnosis date.</a:t>
           </a:r>
         </a:p>
         <a:p>
@@ -14275,8 +14232,8 @@
   </sheetPr>
   <dimension ref="B2:I31"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14752,7 +14709,7 @@
         <v>437</v>
       </c>
       <c r="G19" s="89">
-        <v>42552</v>
+        <v>43070</v>
       </c>
       <c r="H19" s="88" t="s">
         <v>410</v>
@@ -14856,7 +14813,7 @@
         <v>437</v>
       </c>
       <c r="G23" s="89">
-        <v>42552</v>
+        <v>43070</v>
       </c>
       <c r="H23" s="88" t="s">
         <v>410</v>
@@ -14882,7 +14839,7 @@
         <v>437</v>
       </c>
       <c r="G24" s="89">
-        <v>42552</v>
+        <v>43070</v>
       </c>
       <c r="H24" s="88" t="s">
         <v>410</v>
@@ -17252,7 +17209,7 @@
   <dimension ref="B1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="I42" sqref="I42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -17295,7 +17252,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="50">
-        <v>42552</v>
+        <v>43070</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -18745,7 +18702,7 @@
   <dimension ref="B1:F20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -18788,7 +18745,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="50">
-        <v>42705</v>
+        <v>43070</v>
       </c>
     </row>
     <row r="6" spans="2:6" ht="30" x14ac:dyDescent="0.25">
@@ -19008,8 +18965,8 @@
   </sheetPr>
   <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -19052,7 +19009,7 @@
         <v>31</v>
       </c>
       <c r="C5" s="50">
-        <v>42552</v>
+        <v>43070</v>
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.3">
@@ -19982,7 +19939,7 @@
   </sheetPr>
   <dimension ref="B1:F18"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+    <sheetView topLeftCell="A17" workbookViewId="0">
       <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>

</xml_diff>